<commit_message>
Add gestion des risques
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenthardouin/OneDrive - Université de Tours/Projet GL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenthardouin/Documents/L2 INFO/Projet_GL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165A3961-A46C-8D49-A8A4-A35664B15F6D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF28734-2FA0-184A-BABF-773389CD28DF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" xr2:uid="{CA312187-1D2B-3547-9A65-F5E78FBB1065}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="81">
   <si>
     <t>n° taches</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Definir caractéristiqes emploi du temps</t>
   </si>
   <si>
-    <t>Affichage en fonction des droits</t>
-  </si>
-  <si>
     <t>Base de données 1 : info fillière</t>
   </si>
   <si>
@@ -90,24 +87,9 @@
     <t>Class définissant toutes les DROLLS</t>
   </si>
   <si>
-    <t>Gérer les droits d'accès</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Class de connexion, de définition des droits </t>
-  </si>
-  <si>
-    <t>User Interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Programmation de l'interface visuels final </t>
-  </si>
-  <si>
     <t>Aide à la réalisation des emplois du temps</t>
   </si>
   <si>
-    <t xml:space="preserve">Réfléchir à l'affichage </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sprint 1 </t>
   </si>
   <si>
@@ -204,9 +186,6 @@
     <t>Connexion/ deconnexion</t>
   </si>
   <si>
-    <t>App permettant la connexion et le deconnexion à l'application avec interface visuel</t>
-  </si>
-  <si>
     <t>Doc de la class Connexion</t>
   </si>
   <si>
@@ -270,19 +249,25 @@
     <t>6.P</t>
   </si>
   <si>
-    <t>Affichage et Reliage</t>
-  </si>
-  <si>
-    <t>App permettant l'affichage et la connexion entre les class</t>
-  </si>
-  <si>
     <t>6.T</t>
   </si>
   <si>
-    <t>Tests de l'affichage sur différentes tailles , systemes etc.</t>
-  </si>
-  <si>
-    <t>Doc affichage</t>
+    <t>Droits d'accès</t>
+  </si>
+  <si>
+    <t>Class permettant d'établir les différents droits</t>
+  </si>
+  <si>
+    <t>Doc de la class Droits</t>
+  </si>
+  <si>
+    <t>Sprint 7</t>
+  </si>
+  <si>
+    <t>7.P</t>
+  </si>
+  <si>
+    <t>App permettant la connexion / deconnexion et ajout d'un user :  app avec interface visuel</t>
   </si>
 </sst>
 </file>
@@ -427,8 +412,8 @@
     <cellStyle name="60 % - Accent3" xfId="2" builtinId="40"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Style 1" xfId="3" xr:uid="{BE4D2AD5-3BFF-6747-90F8-D4571CA67FE8}"/>
-    <cellStyle name="Style 2" xfId="4" xr:uid="{348BD403-8689-6F45-A862-C6C74B31A26D}"/>
+    <cellStyle name="Style 1 univ" xfId="3" xr:uid="{BE4D2AD5-3BFF-6747-90F8-D4571CA67FE8}"/>
+    <cellStyle name="Style 2 univ" xfId="4" xr:uid="{348BD403-8689-6F45-A862-C6C74B31A26D}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -535,8 +520,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CDD292A9-21F8-D942-8496-D08A23699AF5}" name="Tableau3" displayName="Tableau3" ref="I7:K27" totalsRowShown="0" dataDxfId="3" headerRowCellStyle="Style 1">
-  <autoFilter ref="I7:K27" xr:uid="{B30DE539-5C64-3642-95D1-B5B37C7B5119}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CDD292A9-21F8-D942-8496-D08A23699AF5}" name="Tableau3" displayName="Tableau3" ref="I7:K34" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="I7:K34" xr:uid="{B30DE539-5C64-3642-95D1-B5B37C7B5119}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{34ED2E96-4161-DC40-9181-877512376F9D}" name="Tâches" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{AAC696A6-8F77-9940-8D51-3DB09A4C68F5}" name="Antériorité" dataDxfId="1"/>
@@ -843,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54406A8-5F10-3F49-A1F9-904528393ED2}">
-  <dimension ref="B1:K44"/>
+  <dimension ref="B1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="92" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -861,7 +846,7 @@
   <sheetData>
     <row r="1" spans="2:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C1" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -869,7 +854,7 @@
     <row r="2" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -878,7 +863,7 @@
     </row>
     <row r="4" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -887,7 +872,7 @@
     </row>
     <row r="5" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -905,177 +890,183 @@
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9">
         <f>SUM(F9:F13)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G8" s="7"/>
       <c r="I8" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="K8" s="1">
+        <f>F9</f>
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1">
         <v>2</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K9" s="1">
+        <f t="shared" ref="K9:K12" si="0">F10</f>
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="K10" s="1">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="1">
         <v>4</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="K11" s="1">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="K12" s="1">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="K13" s="1">
+        <f>F15</f>
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="7"/>
       <c r="C14" s="7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
@@ -1085,123 +1076,128 @@
       </c>
       <c r="G14" s="7"/>
       <c r="I14" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="K14" s="1">
+        <f t="shared" ref="K14:K16" si="1">F16</f>
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" s="1">
         <v>3</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K15" s="1">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" s="1">
         <v>10</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="K16" s="1">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F17" s="1">
         <v>4</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="K17" s="1">
+        <f>F20</f>
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F18" s="1">
         <v>10</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="K18" s="1">
+        <f t="shared" ref="K18:K19" si="2">F21</f>
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="8"/>
@@ -1211,97 +1207,101 @@
       </c>
       <c r="G19" s="7"/>
       <c r="I19" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="K19" s="1">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
         <v>10</v>
       </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" s="1">
         <v>4</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="K20" s="1">
+        <f>F24</f>
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" s="1">
         <v>7</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="K21" s="1">
+        <f t="shared" ref="K21:K22" si="3">F25</f>
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F22" s="1">
         <v>3</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="K22" s="1">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="8"/>
@@ -1311,91 +1311,101 @@
       </c>
       <c r="G23" s="7"/>
       <c r="I23" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K23" s="1">
+        <f>F28</f>
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
         <v>18</v>
       </c>
-      <c r="D24" t="s">
-        <v>19</v>
-      </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" s="1">
         <v>7</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="K24" s="1">
+        <f t="shared" ref="K24:K25" si="4">F29</f>
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F25" s="1">
         <v>3</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="K25" s="1">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F26" s="1">
         <v>5</v>
       </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" s="1">
+        <f>F32</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="8"/>
@@ -1404,170 +1414,188 @@
         <v>13</v>
       </c>
       <c r="G27" s="7"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
+      <c r="I27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" ref="K27:K28" si="5">F33</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" s="1">
         <v>5</v>
       </c>
+      <c r="I28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E29" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F29" s="1">
         <v>3</v>
       </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E30" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F30" s="1">
         <v>5</v>
       </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="F31" s="9">
+        <f>SUM(F32:F34)</f>
+        <v>13</v>
+      </c>
       <c r="G31" s="7"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="F32" s="1">
+        <v>4</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="1">
+        <v>6</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>79</v>
       </c>
-      <c r="C33" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" t="s">
-        <v>84</v>
-      </c>
-      <c r="E34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="F37" s="1"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="E39" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F39" s="9">
-        <f>SUM(F8,F14,F19,F23,F27)</f>
-        <v>83</v>
+        <f>SUM(F8,F14,F19,F23,F27,F31)</f>
+        <v>98</v>
       </c>
       <c r="G39" s="7"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C42" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" t="s">
-        <v>22</v>
-      </c>
-      <c r="E42" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C43" t="s">
-        <v>23</v>
-      </c>
-      <c r="D43" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" t="s">
-        <v>26</v>
-      </c>
-      <c r="E44" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44">
-        <v>60</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>